<commit_message>
Fix conversion factor in conversion_factors.xlsx. MW to kW = 0.001, not 0.01.
</commit_message>
<xml_diff>
--- a/premise/data/metals/activities_mapping.xlsx
+++ b/premise/data/metals/activities_mapping.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B620114-71CD-8A4D-B365-695A27388BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A220F7-B88E-D04F-BA36-82DBA5E6178F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities_mapping" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">activities_mapping!$A$1:$K$309</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1563,10 +1566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E213" sqref="E213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1619,7 +1623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1645,7 +1649,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1671,7 +1675,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1697,7 +1701,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1723,7 +1727,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1749,7 +1753,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1775,7 +1779,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1801,7 +1805,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1827,7 +1831,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1879,7 +1883,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1905,7 +1909,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -1937,7 +1941,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1964,7 +1968,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2042,7 +2046,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2068,7 +2072,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2094,7 +2098,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -2120,7 +2124,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2146,7 +2150,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2172,7 +2176,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2198,7 +2202,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2224,7 +2228,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2250,7 +2254,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2276,7 +2280,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2302,7 +2306,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2357,7 +2361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2383,7 +2387,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -2446,7 +2450,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -2473,7 +2477,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -2500,7 +2504,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -2560,7 +2564,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -2589,7 +2593,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -2615,7 +2619,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2645,7 +2649,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -2675,7 +2679,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2705,7 +2709,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2735,7 +2739,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -2765,7 +2769,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -2795,7 +2799,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -2825,7 +2829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>357</v>
       </c>
@@ -2855,7 +2859,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -2885,7 +2889,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -2915,7 +2919,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -2945,7 +2949,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -2974,7 +2978,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -3000,7 +3004,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -3030,7 +3034,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -3060,7 +3064,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -3108,7 +3112,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -3132,7 +3136,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -3156,7 +3160,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -3167,7 +3171,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -3196,7 +3200,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>91</v>
       </c>
@@ -3255,7 +3259,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -3285,7 +3289,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>27</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -3357,7 +3361,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>343</v>
       </c>
@@ -3393,7 +3397,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -3429,7 +3433,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>30</v>
       </c>
@@ -3459,7 +3463,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>99</v>
       </c>
@@ -3495,7 +3499,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -3521,7 +3525,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>37</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>357</v>
       </c>
@@ -3573,7 +3577,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="D72" s="3" t="s">
         <v>102</v>
       </c>
@@ -3584,7 +3588,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -3614,7 +3618,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -3644,7 +3648,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -3674,7 +3678,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -3734,7 +3738,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -3764,7 +3768,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -3794,7 +3798,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -3824,7 +3828,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -3854,7 +3858,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -3884,7 +3888,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -3911,7 +3915,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>34</v>
       </c>
@@ -3938,7 +3942,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>35</v>
       </c>
@@ -3965,7 +3969,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -3991,7 +3995,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -4017,7 +4021,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>21</v>
       </c>
@@ -4046,7 +4050,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -4075,7 +4079,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -4101,7 +4105,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -4127,7 +4131,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -4153,7 +4157,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>27</v>
       </c>
@@ -4189,7 +4193,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>28</v>
       </c>
@@ -4222,7 +4226,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>29</v>
       </c>
@@ -4255,7 +4259,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>30</v>
       </c>
@@ -4288,7 +4292,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>37</v>
       </c>
@@ -4314,7 +4318,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -4340,7 +4344,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4366,7 +4370,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -4392,7 +4396,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>20</v>
       </c>
@@ -4418,7 +4422,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>21</v>
       </c>
@@ -4444,7 +4448,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>22</v>
       </c>
@@ -4470,7 +4474,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>25</v>
       </c>
@@ -4522,7 +4526,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -4552,7 +4556,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -4582,7 +4586,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>34</v>
       </c>
@@ -4612,7 +4616,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>35</v>
       </c>
@@ -4642,7 +4646,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>36</v>
       </c>
@@ -4672,7 +4676,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>341</v>
       </c>
@@ -4702,7 +4706,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>156</v>
       </c>
@@ -4728,7 +4732,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>19</v>
       </c>
@@ -4754,7 +4758,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>20</v>
       </c>
@@ -4780,7 +4784,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>339</v>
       </c>
@@ -4806,7 +4810,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>25</v>
       </c>
@@ -4832,7 +4836,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>10</v>
       </c>
@@ -4862,7 +4866,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>15</v>
       </c>
@@ -4892,7 +4896,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>91</v>
       </c>
@@ -4907,7 +4911,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>26</v>
       </c>
@@ -4937,7 +4941,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>27</v>
       </c>
@@ -4973,7 +4977,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>28</v>
       </c>
@@ -5009,7 +5013,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>343</v>
       </c>
@@ -5045,7 +5049,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>29</v>
       </c>
@@ -5078,7 +5082,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>30</v>
       </c>
@@ -5114,7 +5118,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>31</v>
       </c>
@@ -5129,7 +5133,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>32</v>
       </c>
@@ -5144,7 +5148,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>33</v>
       </c>
@@ -5159,7 +5163,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>23</v>
       </c>
@@ -5188,7 +5192,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>24</v>
       </c>
@@ -5214,7 +5218,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>10</v>
       </c>
@@ -5240,7 +5244,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>156</v>
       </c>
@@ -5266,7 +5270,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>183</v>
       </c>
@@ -5292,7 +5296,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>184</v>
       </c>
@@ -5318,7 +5322,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>23</v>
       </c>
@@ -5353,7 +5357,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>24</v>
       </c>
@@ -5388,7 +5392,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>26</v>
       </c>
@@ -5402,7 +5406,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>27</v>
       </c>
@@ -5438,7 +5442,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>28</v>
       </c>
@@ -5474,7 +5478,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>343</v>
       </c>
@@ -5510,7 +5514,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>29</v>
       </c>
@@ -5536,7 +5540,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>30</v>
       </c>
@@ -5562,7 +5566,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>34</v>
       </c>
@@ -5591,7 +5595,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>36</v>
       </c>
@@ -5617,7 +5621,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>341</v>
       </c>
@@ -5643,7 +5647,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>25</v>
       </c>
@@ -5669,7 +5673,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>10</v>
       </c>
@@ -5695,7 +5699,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>15</v>
       </c>
@@ -5721,7 +5725,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>156</v>
       </c>
@@ -5747,7 +5751,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>183</v>
       </c>
@@ -5773,7 +5777,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>184</v>
       </c>
@@ -5799,7 +5803,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>20</v>
       </c>
@@ -5825,7 +5829,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>21</v>
       </c>
@@ -5851,7 +5855,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>22</v>
       </c>
@@ -5877,7 +5881,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>23</v>
       </c>
@@ -5903,7 +5907,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>24</v>
       </c>
@@ -5929,7 +5933,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>34</v>
       </c>
@@ -5955,7 +5959,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>36</v>
       </c>
@@ -5981,7 +5985,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>25</v>
       </c>
@@ -6007,7 +6011,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -6037,7 +6041,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>15</v>
       </c>
@@ -6073,7 +6077,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>156</v>
       </c>
@@ -6103,7 +6107,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>183</v>
       </c>
@@ -6133,7 +6137,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>184</v>
       </c>
@@ -6163,7 +6167,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>156</v>
       </c>
@@ -6177,7 +6181,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>183</v>
       </c>
@@ -6191,7 +6195,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>184</v>
       </c>
@@ -6205,7 +6209,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -6234,7 +6238,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>20</v>
       </c>
@@ -6263,7 +6267,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>22</v>
       </c>
@@ -6292,7 +6296,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>23</v>
       </c>
@@ -6327,7 +6331,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>24</v>
       </c>
@@ -6362,7 +6366,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>91</v>
       </c>
@@ -6388,7 +6392,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>26</v>
       </c>
@@ -6414,7 +6418,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>27</v>
       </c>
@@ -6450,7 +6454,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>28</v>
       </c>
@@ -6483,7 +6487,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>343</v>
       </c>
@@ -6516,7 +6520,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>29</v>
       </c>
@@ -6549,7 +6553,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>30</v>
       </c>
@@ -6575,7 +6579,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>31</v>
       </c>
@@ -6601,7 +6605,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>99</v>
       </c>
@@ -6627,7 +6631,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>32</v>
       </c>
@@ -6641,7 +6645,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>33</v>
       </c>
@@ -6655,7 +6659,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>34</v>
       </c>
@@ -6684,7 +6688,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>36</v>
       </c>
@@ -6698,7 +6702,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>37</v>
       </c>
@@ -6727,7 +6731,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>341</v>
       </c>
@@ -6756,7 +6760,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>25</v>
       </c>
@@ -6782,7 +6786,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>10</v>
       </c>
@@ -6809,7 +6813,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>15</v>
       </c>
@@ -6836,7 +6840,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>156</v>
       </c>
@@ -6863,7 +6867,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>183</v>
       </c>
@@ -6890,7 +6894,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>184</v>
       </c>
@@ -6917,7 +6921,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>23</v>
       </c>
@@ -6944,7 +6948,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>24</v>
       </c>
@@ -6971,7 +6975,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>25</v>
       </c>
@@ -6998,7 +7002,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
         <v>10</v>
       </c>
@@ -7034,7 +7038,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
         <v>10</v>
       </c>
@@ -7070,7 +7074,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>15</v>
       </c>
@@ -7096,7 +7100,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>34</v>
       </c>
@@ -7122,7 +7126,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>36</v>
       </c>
@@ -7148,7 +7152,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>27</v>
       </c>
@@ -7187,7 +7191,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>28</v>
       </c>
@@ -7223,7 +7227,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>29</v>
       </c>
@@ -7256,7 +7260,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>30</v>
       </c>
@@ -7292,7 +7296,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>31</v>
       </c>
@@ -7325,7 +7329,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
         <v>10</v>
       </c>
@@ -7361,7 +7365,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
         <v>10</v>
       </c>
@@ -7397,7 +7401,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>15</v>
       </c>
@@ -7452,7 +7456,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>34</v>
       </c>
@@ -7481,7 +7485,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>36</v>
       </c>
@@ -7539,7 +7543,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>37</v>
       </c>
@@ -7598,7 +7602,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>37</v>
       </c>
@@ -7628,7 +7632,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>10</v>
       </c>
@@ -7658,7 +7662,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>15</v>
       </c>
@@ -7688,7 +7692,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>156</v>
       </c>
@@ -7718,7 +7722,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>184</v>
       </c>
@@ -7748,7 +7752,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>341</v>
       </c>
@@ -7778,7 +7782,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>10</v>
       </c>
@@ -7805,7 +7809,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>10</v>
       </c>
@@ -7831,7 +7835,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>15</v>
       </c>
@@ -7857,7 +7861,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>10</v>
       </c>
@@ -7909,7 +7913,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>10</v>
       </c>
@@ -7939,7 +7943,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>15</v>
       </c>
@@ -7966,7 +7970,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>10</v>
       </c>
@@ -7996,7 +8000,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>15</v>
       </c>
@@ -8023,7 +8027,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>35</v>
       </c>
@@ -8050,7 +8054,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>266</v>
       </c>
@@ -8077,7 +8081,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>21</v>
       </c>
@@ -8103,7 +8107,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>19</v>
       </c>
@@ -8117,7 +8121,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>22</v>
       </c>
@@ -8131,7 +8135,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>23</v>
       </c>
@@ -8142,7 +8146,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>24</v>
       </c>
@@ -8153,7 +8157,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -8179,7 +8183,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>19</v>
       </c>
@@ -8205,7 +8209,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>20</v>
       </c>
@@ -8231,7 +8235,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>21</v>
       </c>
@@ -8257,7 +8261,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>276</v>
       </c>
@@ -8283,7 +8287,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>23</v>
       </c>
@@ -8309,7 +8313,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>277</v>
       </c>
@@ -8335,7 +8339,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>24</v>
       </c>
@@ -8361,7 +8365,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>37</v>
       </c>
@@ -8387,7 +8391,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>25</v>
       </c>
@@ -8413,7 +8417,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>27</v>
       </c>
@@ -8427,7 +8431,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>10</v>
       </c>
@@ -8457,7 +8461,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>341</v>
       </c>
@@ -8487,7 +8491,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>10</v>
       </c>
@@ -8513,7 +8517,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>15</v>
       </c>
@@ -8539,7 +8543,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>10</v>
       </c>
@@ -8565,7 +8569,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>10</v>
       </c>
@@ -8595,7 +8599,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>15</v>
       </c>
@@ -8622,7 +8626,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>156</v>
       </c>
@@ -8649,7 +8653,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>183</v>
       </c>
@@ -8676,7 +8680,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>184</v>
       </c>
@@ -8703,7 +8707,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>10</v>
       </c>
@@ -8729,7 +8733,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>19</v>
       </c>
@@ -8758,7 +8762,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>20</v>
       </c>
@@ -8787,7 +8791,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>21</v>
       </c>
@@ -8816,7 +8820,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>22</v>
       </c>
@@ -8845,7 +8849,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>25</v>
       </c>
@@ -8871,7 +8875,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>23</v>
       </c>
@@ -8897,7 +8901,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>24</v>
       </c>
@@ -8923,7 +8927,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>30</v>
       </c>
@@ -8952,7 +8956,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>31</v>
       </c>
@@ -9007,7 +9011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>10</v>
       </c>
@@ -9037,7 +9041,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>25</v>
       </c>
@@ -9067,7 +9071,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>156</v>
       </c>
@@ -9097,7 +9101,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>184</v>
       </c>
@@ -9127,7 +9131,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>23</v>
       </c>
@@ -9157,7 +9161,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>24</v>
       </c>
@@ -9187,7 +9191,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>99</v>
       </c>
@@ -9217,7 +9221,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>25</v>
       </c>
@@ -9247,7 +9251,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>10</v>
       </c>
@@ -9277,7 +9281,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>15</v>
       </c>
@@ -9307,7 +9311,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>10</v>
       </c>
@@ -9337,7 +9341,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>15</v>
       </c>
@@ -9364,7 +9368,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>327</v>
       </c>
@@ -9391,7 +9395,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>36</v>
       </c>
@@ -9418,7 +9422,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>25</v>
       </c>
@@ -9445,7 +9449,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>341</v>
       </c>
@@ -9472,7 +9476,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>183</v>
       </c>
@@ -9501,7 +9505,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>184</v>
       </c>
@@ -9530,7 +9534,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>19</v>
       </c>
@@ -9556,7 +9560,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>21</v>
       </c>
@@ -9585,7 +9589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>23</v>
       </c>
@@ -9614,7 +9618,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>24</v>
       </c>
@@ -9643,7 +9647,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>36</v>
       </c>
@@ -9669,7 +9673,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>10</v>
       </c>
@@ -9699,7 +9703,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>35</v>
       </c>
@@ -9726,7 +9730,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>36</v>
       </c>
@@ -9756,7 +9760,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>37</v>
       </c>
@@ -9786,7 +9790,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>341</v>
       </c>
@@ -9816,7 +9820,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>25</v>
       </c>
@@ -9843,7 +9847,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>32</v>
       </c>
@@ -9879,7 +9883,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>32</v>
       </c>
@@ -9915,7 +9919,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>32</v>
       </c>
@@ -9951,7 +9955,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>32</v>
       </c>
@@ -9965,7 +9969,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>32</v>
       </c>
@@ -9976,7 +9980,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>32</v>
       </c>
@@ -10002,7 +10006,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>33</v>
       </c>
@@ -10032,7 +10036,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>33</v>
       </c>
@@ -10059,7 +10063,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>33</v>
       </c>
@@ -10070,7 +10074,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>33</v>
       </c>
@@ -10081,7 +10085,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>33</v>
       </c>
@@ -10108,6 +10112,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K309" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="PEMEL"/>
+        <filter val="PEMFC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix typo - Germanium in aSi PV
</commit_message>
<xml_diff>
--- a/premise/data/metals/activities_mapping.xlsx
+++ b/premise/data/metals/activities_mapping.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7EAD9B-9E6E-444F-8006-7501E7C3F4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664497F5-AE29-47E4-85C0-5108202E4B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:M309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A285" sqref="A285"/>
+      <selection activeCell="E279" sqref="E279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4044,7 +4044,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>128</v>
       </c>
       <c r="E90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="s">
         <v>129</v>
@@ -10113,6 +10113,7 @@
   <autoFilter ref="A1:K309" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
+        <filter val="Germanium"/>
         <filter val="Yttrium"/>
       </filters>
     </filterColumn>

</xml_diff>